<commit_message>
phonon and quantum calculation
</commit_message>
<xml_diff>
--- a/diamond/data/diamond_data.xlsx
+++ b/diamond/data/diamond_data.xlsx
@@ -4,13 +4,16 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19890" windowHeight="8370" tabRatio="719"/>
+    <workbookView windowWidth="19890" windowHeight="7950" tabRatio="719"/>
   </bookViews>
   <sheets>
     <sheet name="CCmd" sheetId="1" r:id="rId1"/>
+    <sheet name="draft-phonon" sheetId="2" r:id="rId2"/>
+    <sheet name="draft-QM" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="ExternalData_1" localSheetId="0">CCmd!$D$2:$D$10</definedName>
+    <definedName name="ExternalData_1" localSheetId="1">'draft-phonon'!$B$1:$B$9</definedName>
   </definedNames>
   <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
@@ -18,35 +21,42 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="QM" type="6" background="1" refreshedVersion="2" saveData="1">
+  <connection id="1" name="PN" type="6" background="1" refreshedVersion="2" saveData="1">
+    <textPr sourceFile="F:\William\diamond\PBE3\PN.txt">
+      <textFields>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="2" name="QM" type="6" background="1" refreshedVersion="2" saveData="1">
     <textPr sourceFile="F:\William\diamond\PBE3\QM.txt">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="2" name="tmp1" type="6" background="1" refreshedVersion="2" saveData="1">
+  <connection id="3" name="tmp1" type="6" background="1" refreshedVersion="2" saveData="1">
     <textPr sourceFile="F:\William\tmp\tmp.txt">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="3" name="tmp2" type="6" background="1" refreshedVersion="2" saveData="1">
+  <connection id="4" name="tmp2" type="6" background="1" refreshedVersion="2" saveData="1">
     <textPr sourceFile="F:\William\PV0c\tmp.txt" space="1" consecutive="1">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="4" name="tmpp1" type="6" background="1" refreshedVersion="2" saveData="1">
+  <connection id="5" name="tmpp1" type="6" background="1" refreshedVersion="2" saveData="1">
     <textPr sourceFile="F:\William\PV0c\tmpp.txt" space="1" consecutive="1">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="5" name="tmpt2" type="6" background="1" refreshedVersion="2" saveData="1">
+  <connection id="6" name="tmpt2" type="6" background="1" refreshedVersion="2" saveData="1">
     <textPr sourceFile="F:\William\PBEnew\tmpt.txt">
       <textFields>
         <textField/>
@@ -57,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13">
   <si>
     <t>V%</t>
   </si>
@@ -66,6 +76,9 @@
   </si>
   <si>
     <t>QM</t>
+  </si>
+  <si>
+    <t>PN</t>
   </si>
   <si>
     <t>a</t>
@@ -100,9 +113,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="21">
@@ -115,6 +128,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -122,6 +142,21 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -130,9 +165,16 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -144,84 +186,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -233,8 +202,53 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -249,17 +263,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -274,19 +287,127 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -298,31 +419,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -334,61 +431,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -400,61 +467,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -465,39 +478,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -531,13 +511,35 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
-      <top style="thin">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -565,151 +567,162 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="28" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -778,6 +791,16 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ExternalData_1" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+  <queryTableRefresh preserveSortFilterLayout="0" nextId="2">
+    <queryTableFields count="1">
+      <queryTableField id="1" dataBound="0"/>
+    </queryTableFields>
+  </queryTableRefresh>
+</queryTable>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ExternalData_1" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh preserveSortFilterLayout="0" nextId="2">
     <queryTableFields count="1">
@@ -1045,13 +1068,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="2" width="9" style="1"/>
     <col min="3" max="3" width="19.125" style="1" customWidth="1"/>
@@ -1059,7 +1082,7 @@
     <col min="5" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4">
+    <row r="1" spans="2:5">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1069,10 +1092,13 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1">
         <v>1.06</v>
@@ -1081,13 +1107,16 @@
         <f>POWER(B2,1/3)</f>
         <v>1.01961282242222</v>
       </c>
-      <c r="D2" s="2">
-        <v>-18.143411</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="D2">
+        <v>-9.0717055</v>
+      </c>
+      <c r="E2">
+        <v>0.0189873289115637</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3" s="1">
         <v>1.04</v>
@@ -1096,13 +1125,16 @@
         <f>B3^(1/3)</f>
         <v>1.01315940382018</v>
       </c>
-      <c r="D3" s="2">
-        <v>-18.228197</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="D3">
+        <v>-9.1140985</v>
+      </c>
+      <c r="E3">
+        <v>0.0193641677609261</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4" s="1">
         <v>1.02</v>
@@ -1111,13 +1143,16 @@
         <f t="shared" ref="C3:C10" si="0">POWER(B4,1/3)</f>
         <v>1.00662270956011</v>
       </c>
-      <c r="D4" s="2">
-        <v>-18.306019</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="D4">
+        <v>-9.1530095</v>
+      </c>
+      <c r="E4">
+        <v>0.0197557853423853</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B5" s="1">
         <v>1</v>
@@ -1126,13 +1161,16 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="D5" s="2">
-        <v>-18.376018</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="D5">
+        <v>-9.188009</v>
+      </c>
+      <c r="E5">
+        <v>0.0201579055402523</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B6" s="1">
         <v>0.98</v>
@@ -1141,13 +1179,16 @@
         <f t="shared" si="0"/>
         <v>0.993288388379269</v>
       </c>
-      <c r="D6" s="2">
-        <v>-18.437319</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="D6">
+        <v>-9.2186595</v>
+      </c>
+      <c r="E6">
+        <v>0.0205726748987848</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B7" s="1">
         <v>0.96</v>
@@ -1156,13 +1197,16 @@
         <f t="shared" si="0"/>
         <v>0.986484829732188</v>
       </c>
-      <c r="D7" s="2">
-        <v>-18.488905</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="D7">
+        <v>-9.2444525</v>
+      </c>
+      <c r="E7">
+        <v>0.0210006087570371</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B8" s="1">
         <v>0.94</v>
@@ -1171,13 +1215,16 @@
         <f t="shared" si="0"/>
         <v>0.979586108715562</v>
       </c>
-      <c r="D8" s="2">
-        <v>-18.529689</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="D8">
+        <v>-9.2648445</v>
+      </c>
+      <c r="E8">
+        <v>0.0214412456743952</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B9" s="1">
         <v>0.92</v>
@@ -1186,13 +1233,16 @@
         <f t="shared" si="0"/>
         <v>0.972588826218856</v>
       </c>
-      <c r="D9" s="2">
-        <v>-18.558455</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="D9">
+        <v>-9.2792275</v>
+      </c>
+      <c r="E9">
+        <v>0.0218967518239959</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B10" s="1">
         <v>0.9</v>
@@ -1201,8 +1251,268 @@
         <f t="shared" si="0"/>
         <v>0.96548938460563</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10">
+        <v>-9.2869315</v>
+      </c>
+      <c r="E10">
+        <v>0.0223664061846353</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" outlineLevelCol="2"/>
+  <cols>
+    <col min="2" max="2" width="11.5" customWidth="1"/>
+    <col min="3" max="3" width="12.625"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1">
+        <v>29.3096749</v>
+      </c>
+      <c r="C1">
+        <f>B1*1000/6.022140857E+23*6242000000000000000/16</f>
+        <v>0.0189873289115637</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>29.8913799</v>
+      </c>
+      <c r="C2">
+        <f t="shared" ref="C2:C9" si="0">B2*1000/6.022140857E+23*6242000000000000000/16</f>
+        <v>0.0193641677609261</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <v>30.495898</v>
+      </c>
+      <c r="C3">
+        <f t="shared" si="0"/>
+        <v>0.0197557853423853</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>31.1166284</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>0.0201579055402523</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>31.7568846</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>0.0205726748987848</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>32.4174621</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>0.0210006087570371</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7">
+        <v>33.0976486</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>0.0214412456743952</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <v>33.8007879</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>0.0218967518239959</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9">
+        <v>34.525767</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>0.0223664061846353</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" outlineLevelCol="2"/>
+  <cols>
+    <col min="3" max="3" width="11.5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="2">
+        <v>-18.143411</v>
+      </c>
+      <c r="C1">
+        <f>B1/2</f>
+        <v>-9.0717055</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2">
+        <v>-18.228197</v>
+      </c>
+      <c r="C2">
+        <f t="shared" ref="C2:C9" si="0">B2/2</f>
+        <v>-9.1140985</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2">
+        <v>-18.306019</v>
+      </c>
+      <c r="C3">
+        <f t="shared" si="0"/>
+        <v>-9.1530095</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="2">
+        <v>-18.376018</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>-9.188009</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="2">
+        <v>-18.437319</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>-9.2186595</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="2">
+        <v>-18.488905</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>-9.2444525</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="2">
+        <v>-18.529689</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>-9.2648445</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="2">
+        <v>-18.558455</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>-9.2792275</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="2">
         <v>-18.573863</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>-9.2869315</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
collect data for QM and phonons
</commit_message>
<xml_diff>
--- a/diamond/data/diamond_data.xlsx
+++ b/diamond/data/diamond_data.xlsx
@@ -67,18 +67,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17">
   <si>
-    <t>V%</t>
+    <t>V</t>
   </si>
   <si>
-    <t>a%</t>
+    <t>vol ratio</t>
   </si>
   <si>
     <t>QM</t>
   </si>
   <si>
     <t>PN</t>
+  </si>
+  <si>
+    <t>QMPN</t>
   </si>
   <si>
     <t>a</t>
@@ -107,14 +110,23 @@
   <si>
     <t>z06</t>
   </si>
+  <si>
+    <t>QM/2</t>
+  </si>
+  <si>
+    <t>vol%</t>
+  </si>
+  <si>
+    <t>vol</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
@@ -127,22 +139,69 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -156,10 +215,19 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -172,46 +240,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -226,45 +255,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -277,6 +275,20 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -287,187 +299,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -481,32 +493,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -526,29 +517,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -570,6 +549,39 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -581,148 +593,148 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="26" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1068,21 +1080,23 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" outlineLevelCol="5"/>
   <cols>
     <col min="1" max="2" width="9" style="1"/>
     <col min="3" max="3" width="19.125" style="1" customWidth="1"/>
     <col min="4" max="4" width="12.625" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9" style="1"/>
+    <col min="5" max="5" width="9" style="1"/>
+    <col min="6" max="6" width="13.75" style="1"/>
+    <col min="7" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5">
+    <row r="1" spans="2:6">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1095,17 +1109,19 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="1">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>6.7115278</v>
+      </c>
+      <c r="C2" s="1">
         <v>1.06</v>
-      </c>
-      <c r="C2" s="1">
-        <f>POWER(B2,1/3)</f>
-        <v>1.01961282242222</v>
       </c>
       <c r="D2">
         <v>-9.0717055</v>
@@ -1113,17 +1129,20 @@
       <c r="E2">
         <v>0.0189873289115637</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2" s="1">
+        <f>D2+E2</f>
+        <v>-9.05271817108844</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="1">
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <v>6.5848952</v>
+      </c>
+      <c r="C3" s="1">
         <v>1.04</v>
-      </c>
-      <c r="C3" s="1">
-        <f>B3^(1/3)</f>
-        <v>1.01315940382018</v>
       </c>
       <c r="D3">
         <v>-9.1140985</v>
@@ -1131,17 +1150,20 @@
       <c r="E3">
         <v>0.0193641677609261</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="F3" s="1">
+        <f t="shared" ref="F3:F10" si="0">D3+E3</f>
+        <v>-9.09473433223907</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="1">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>6.4582626</v>
+      </c>
+      <c r="C4" s="1">
         <v>1.02</v>
-      </c>
-      <c r="C4" s="1">
-        <f t="shared" ref="C3:C10" si="0">POWER(B4,1/3)</f>
-        <v>1.00662270956011</v>
       </c>
       <c r="D4">
         <v>-9.1530095</v>
@@ -1149,16 +1171,19 @@
       <c r="E4">
         <v>0.0197557853423853</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="F4" s="1">
+        <f t="shared" si="0"/>
+        <v>-9.13325371465761</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="1">
-        <v>1</v>
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>6.33163</v>
       </c>
       <c r="C5" s="1">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="D5">
@@ -1167,17 +1192,20 @@
       <c r="E5">
         <v>0.0201579055402523</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="F5" s="1">
+        <f t="shared" si="0"/>
+        <v>-9.16785109445975</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="1">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>6.2049974</v>
+      </c>
+      <c r="C6" s="1">
         <v>0.98</v>
-      </c>
-      <c r="C6" s="1">
-        <f t="shared" si="0"/>
-        <v>0.993288388379269</v>
       </c>
       <c r="D6">
         <v>-9.2186595</v>
@@ -1185,17 +1213,20 @@
       <c r="E6">
         <v>0.0205726748987848</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="F6" s="1">
+        <f t="shared" si="0"/>
+        <v>-9.19808682510121</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="1">
+        <v>10</v>
+      </c>
+      <c r="B7">
+        <v>6.0783648</v>
+      </c>
+      <c r="C7" s="1">
         <v>0.96</v>
-      </c>
-      <c r="C7" s="1">
-        <f t="shared" si="0"/>
-        <v>0.986484829732188</v>
       </c>
       <c r="D7">
         <v>-9.2444525</v>
@@ -1203,17 +1234,20 @@
       <c r="E7">
         <v>0.0210006087570371</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="F7" s="1">
+        <f t="shared" si="0"/>
+        <v>-9.22345189124296</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="1">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <v>5.9517322</v>
+      </c>
+      <c r="C8" s="1">
         <v>0.94</v>
-      </c>
-      <c r="C8" s="1">
-        <f t="shared" si="0"/>
-        <v>0.979586108715562</v>
       </c>
       <c r="D8">
         <v>-9.2648445</v>
@@ -1221,17 +1255,20 @@
       <c r="E8">
         <v>0.0214412456743952</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="F8" s="1">
+        <f t="shared" si="0"/>
+        <v>-9.2434032543256</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="1">
+        <v>12</v>
+      </c>
+      <c r="B9">
+        <v>5.8250996</v>
+      </c>
+      <c r="C9" s="1">
         <v>0.92</v>
-      </c>
-      <c r="C9" s="1">
-        <f t="shared" si="0"/>
-        <v>0.972588826218856</v>
       </c>
       <c r="D9">
         <v>-9.2792275</v>
@@ -1239,23 +1276,30 @@
       <c r="E9">
         <v>0.0218967518239959</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="F9" s="1">
+        <f t="shared" si="0"/>
+        <v>-9.257330748176</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="1">
+        <v>13</v>
+      </c>
+      <c r="B10">
+        <v>5.698467</v>
+      </c>
+      <c r="C10" s="1">
         <v>0.9</v>
-      </c>
-      <c r="C10" s="1">
-        <f t="shared" si="0"/>
-        <v>0.96548938460563</v>
       </c>
       <c r="D10">
         <v>-9.2869315</v>
       </c>
       <c r="E10">
         <v>0.0223664061846353</v>
+      </c>
+      <c r="F10" s="1">
+        <f t="shared" si="0"/>
+        <v>-9.26456509381536</v>
       </c>
     </row>
   </sheetData>
@@ -1281,7 +1325,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B1">
         <v>29.3096749</v>
@@ -1293,7 +1337,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2">
         <v>29.8913799</v>
@@ -1305,7 +1349,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3">
         <v>30.495898</v>
@@ -1317,7 +1361,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B4">
         <v>31.1166284</v>
@@ -1329,7 +1373,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B5">
         <v>31.7568846</v>
@@ -1341,7 +1385,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B6">
         <v>32.4174621</v>
@@ -1353,7 +1397,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B7">
         <v>33.0976486</v>
@@ -1365,7 +1409,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B8">
         <v>33.8007879</v>
@@ -1377,7 +1421,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B9">
         <v>34.525767</v>
@@ -1396,123 +1440,202 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C9"/>
+      <selection activeCell="D1" sqref="D1:D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" outlineLevelCol="4"/>
   <cols>
+    <col min="2" max="2" width="9.5"/>
     <col min="3" max="3" width="11.5"/>
+    <col min="5" max="5" width="10.375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="2">
-        <v>-18.143411</v>
-      </c>
-      <c r="C1">
-        <f>B1/2</f>
-        <v>-9.0717055</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+    <row r="1" spans="2:5">
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="2">
-        <v>-18.228197</v>
+        <v>-18.143411</v>
       </c>
       <c r="C2">
-        <f t="shared" ref="C2:C9" si="0">B2/2</f>
-        <v>-9.1140985</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <f>B2/2</f>
+        <v>-9.0717055</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1.06</v>
+      </c>
+      <c r="E2">
+        <f>$D2*6.33163</f>
+        <v>6.7115278</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="2">
-        <v>-18.306019</v>
+        <v>-18.228197</v>
       </c>
       <c r="C3">
-        <f t="shared" si="0"/>
-        <v>-9.1530095</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <f t="shared" ref="C3:C10" si="0">B3/2</f>
+        <v>-9.1140985</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1.04</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E10" si="1">$D3*6.33163</f>
+        <v>6.5848952</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="2">
-        <v>-18.376018</v>
+        <v>-18.306019</v>
       </c>
       <c r="C4">
         <f t="shared" si="0"/>
-        <v>-9.188009</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+        <v>-9.1530095</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1.02</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="1"/>
+        <v>6.4582626</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="2">
-        <v>-18.437319</v>
+        <v>-18.376018</v>
       </c>
       <c r="C5">
         <f t="shared" si="0"/>
-        <v>-9.2186595</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>-9.188009</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="1"/>
+        <v>6.33163</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="2">
-        <v>-18.488905</v>
+        <v>-18.437319</v>
       </c>
       <c r="C6">
         <f t="shared" si="0"/>
-        <v>-9.2444525</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+        <v>-9.2186595</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0.98</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="1"/>
+        <v>6.2049974</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B7" s="2">
-        <v>-18.529689</v>
+        <v>-18.488905</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>-9.2648445</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+        <v>-9.2444525</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0.96</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="1"/>
+        <v>6.0783648</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B8" s="2">
-        <v>-18.558455</v>
+        <v>-18.529689</v>
       </c>
       <c r="C8">
         <f t="shared" si="0"/>
-        <v>-9.2792275</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+        <v>-9.2648445</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0.94</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="1"/>
+        <v>5.9517322</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="2">
+        <v>-18.558455</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>-9.2792275</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0.92</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="1"/>
+        <v>5.8250996</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="2">
         <v>-18.573863</v>
       </c>
-      <c r="C9">
+      <c r="C10">
         <f t="shared" si="0"/>
         <v>-9.2869315</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="1"/>
+        <v>5.698467</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
data up to 55% compression and 400 Gpa
</commit_message>
<xml_diff>
--- a/diamond/data/diamond_data.xlsx
+++ b/diamond/data/diamond_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19890" windowHeight="9405" tabRatio="719" activeTab="2"/>
+    <workbookView windowWidth="19890" windowHeight="8985" tabRatio="719"/>
   </bookViews>
   <sheets>
     <sheet name="CCmd" sheetId="1" r:id="rId1"/>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20">
   <si>
     <t>V</t>
   </si>
@@ -109,6 +109,15 @@
   </si>
   <si>
     <t>z06</t>
+  </si>
+  <si>
+    <t>z07</t>
+  </si>
+  <si>
+    <t>z08</t>
+  </si>
+  <si>
+    <t>z09</t>
   </si>
   <si>
     <t>QM/2</t>
@@ -125,9 +134,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="21">
@@ -139,24 +148,11 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -171,14 +167,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -186,6 +175,28 @@
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -198,8 +209,39 @@
     </font>
     <font>
       <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -213,19 +255,25 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -233,14 +281,6 @@
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -252,39 +292,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -299,187 +308,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -496,8 +505,32 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -517,11 +550,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -541,21 +580,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -567,41 +591,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -611,134 +620,134 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -746,6 +755,7 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1080,15 +1090,16 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11:B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="2" width="9" style="1"/>
+    <col min="1" max="1" width="9" style="1"/>
+    <col min="2" max="2" width="9.375" style="1"/>
     <col min="3" max="3" width="19.125" style="1" customWidth="1"/>
     <col min="4" max="4" width="12.625" style="1" customWidth="1"/>
     <col min="5" max="5" width="9" style="1"/>
@@ -1300,6 +1311,57 @@
       <c r="F10" s="1">
         <f t="shared" si="0"/>
         <v>-9.26456509381536</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11">
+        <v>5.3185692</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0.84</v>
+      </c>
+      <c r="D11" s="1">
+        <v>-9.2620585</v>
+      </c>
+      <c r="F11" s="1">
+        <v>-9.2620585</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12">
+        <v>4.3055084</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0.68</v>
+      </c>
+      <c r="D12" s="1">
+        <v>-8.6402785</v>
+      </c>
+      <c r="F12" s="1">
+        <v>-8.6402785</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13">
+        <v>3.4823965</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0.55</v>
+      </c>
+      <c r="D13" s="1">
+        <v>-6.9676815</v>
+      </c>
+      <c r="F13" s="1">
+        <v>-6.9676815</v>
       </c>
     </row>
   </sheetData>
@@ -1442,8 +1504,8 @@
   <sheetPr/>
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11:E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" outlineLevelCol="5"/>
@@ -1459,13 +1521,13 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -1675,27 +1737,69 @@
         <v>0.96548938460563</v>
       </c>
     </row>
-    <row r="11" spans="4:6">
+    <row r="11" spans="1:6">
+      <c r="A11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="3">
+        <v>-18.524117</v>
+      </c>
+      <c r="C11">
+        <f>B11/2</f>
+        <v>-9.2620585</v>
+      </c>
       <c r="D11" s="1">
         <v>0.84</v>
+      </c>
+      <c r="E11">
+        <f>$D11*6.33163</f>
+        <v>5.3185692</v>
       </c>
       <c r="F11">
         <f t="shared" si="2"/>
         <v>0.943538796063307</v>
       </c>
     </row>
-    <row r="12" spans="4:6">
+    <row r="12" spans="1:6">
+      <c r="A12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="3">
+        <v>-17.280557</v>
+      </c>
+      <c r="C12">
+        <f>B12/2</f>
+        <v>-8.6402785</v>
+      </c>
       <c r="D12" s="1">
         <v>0.68</v>
+      </c>
+      <c r="E12">
+        <f>$D12*6.33163</f>
+        <v>4.3055084</v>
       </c>
       <c r="F12">
         <f t="shared" si="2"/>
         <v>0.879365934431636</v>
       </c>
     </row>
-    <row r="13" spans="4:6">
+    <row r="13" spans="1:6">
+      <c r="A13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="3">
+        <v>-13.935363</v>
+      </c>
+      <c r="C13">
+        <f>B13/2</f>
+        <v>-6.9676815</v>
+      </c>
       <c r="D13" s="1">
         <v>0.55</v>
+      </c>
+      <c r="E13">
+        <f>$D13*6.33163</f>
+        <v>3.4823965</v>
       </c>
       <c r="F13">
         <f t="shared" si="2"/>

</xml_diff>